<commit_message>
Definiendo posiciones de patrones
definiendo posiciones físicas de los sprites
</commit_message>
<xml_diff>
--- a/doc/análisis posición en memoria sprites enemigos.xlsx
+++ b/doc/análisis posición en memoria sprites enemigos.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="lista enemigos" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="NSprites" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Daño" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Posiciones" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Posiciones Mapa" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Posiciones Patrones" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="358">
   <si>
     <t xml:space="preserve">Nombre Enemigo</t>
   </si>
@@ -188,6 +189,915 @@
   </si>
   <si>
     <t xml:space="preserve">explosión</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dirección memoria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprites comunes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3800h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_punto_mira_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3820h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_punto_mira_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3840h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_punto_mira_1_mejorado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3860h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_punto_mira_2_mejorado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3880h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_explosion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3900h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3920h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3940h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3960h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3980h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4000h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4020h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4040h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4060h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4080h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4100h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4120h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4140h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4160h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4180h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4200h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4220h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4240h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4260h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4280h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4300h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4320h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4340h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4360h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4380h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4400h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4420h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4440h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4460h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4480h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4500h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4520h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4540h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4560h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4580h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4600h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4620h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4640h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4660h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4680h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4700h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4720h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4740h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4760h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4780h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4800h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4820h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4840h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4860h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4880h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4900h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4920h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4940h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4960h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4980h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5000h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5020h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5040h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5060h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5080h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5100h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5120h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5140h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5160h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5180h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5200h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5220h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5240h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5260h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5280h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5300h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5320h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5340h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5360h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5380h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5400h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5420h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5440h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5460h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5480h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5500h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5520h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5540h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5560h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5580h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5600h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5620h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5640h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5660h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5680h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5700h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5720h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5740h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5760h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5780h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5800h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5820h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5840h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5860h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5880h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5900h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5920h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5940h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5960h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5980h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6000h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6020h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6040h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6060h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6080h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6100h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6120h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6140h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6160h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6180h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6200h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6220h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6240h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6260h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6280h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6300h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6320h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6340h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6360h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6380h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6400h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6420h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6440h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6460h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6480h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6500h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6520h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6540h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6560h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6580h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6600h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6620h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6640h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6660h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6680h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6700h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6720h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6740h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6760h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6780h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6800h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6820h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6840h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6860h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6880h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6900h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6920h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6940h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6960h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6980h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7000h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7020h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7040h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7060h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7080h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7100h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7120h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7140h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7160h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7180h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7200h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7220h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7240h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7260h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7280h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7300h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7320h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7340h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7360h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7380h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7400h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7420h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7440h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7460h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7480h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7500h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7520h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7540h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7560h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7580h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7600h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7620h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7640h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7660h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7680h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7700h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7720h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo1_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi1_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero1_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7740h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo1_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi1_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero1_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7760h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo1_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi1_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero1_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_manoizquierda_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7780h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo1_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi1_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero1_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_manoizquierda_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7800h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo1_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi1_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero1_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_manoizquierda_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7820h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo1_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi1_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero1_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefebeholder_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_manoizquierda_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7840h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo2_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefemurcielago_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefefantasma_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi2_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero2_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefebeholder_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_manoderecha_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7860h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefemurcielago_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefefantasma_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefebeholder_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_manoderecha_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7880h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo2_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefemurcielago_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefefantasma_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi2_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero2_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefebeholder_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_manoderecha_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7900h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo2_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefemurcielago_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefefantasma_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi2_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero2_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefebeholder_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_manoderecha_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7920h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo2_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefemurcielago_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefefantasma_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi2_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero2_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefebeholder_5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_conde_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7940h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo2_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefemurcielago_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefefantasma_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi2_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero2_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefebeholder_6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_conde_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7960h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo2_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefemurcielago_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefefantasma_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi2_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero2_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefebeholder_7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_conde_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7980h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefelobo2_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefemurcielago_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefefantasma_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefezombi2_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefecaballero2_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_jefebeholder_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_conde_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8000h</t>
   </si>
 </sst>
 </file>
@@ -197,11 +1107,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -218,13 +1129,26 @@
       <name val="Arial"/>
       <family val="0"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF333333"/>
+        <bgColor rgb="FF333300"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -261,7 +1185,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -272,6 +1196,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -293,21 +1225,21 @@
   </sheetPr>
   <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="6" style="0" width="7.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="0" width="9.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="4.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="4.97"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -993,7 +1925,7 @@
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1141,7 +2073,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -1160,7 +2092,7 @@
       <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.65"/>
   </cols>
@@ -1344,7 +2276,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
@@ -1363,29 +2295,29 @@
       <selection pane="topLeft" activeCell="Y1" activeCellId="0" sqref="Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="2.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="2.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="2.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="2.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="2.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="2.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="2.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="2.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="2.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="2.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="2.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="2.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="2.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="10.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="10.92"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3135,7 +4067,1435 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I212"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.6"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="0" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="0" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="0" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="0" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="0" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="0" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="0" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="0" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="0" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="0" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="0" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A112" s="0" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="0" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="0" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A115" s="0" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="0" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="0" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="0" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="0" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="0" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="0" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="0" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="0" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A125" s="0" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="0" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="0" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="0" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="0" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="0" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="0" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="0" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="0" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="0" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="0" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="0" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="0" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="0" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="0" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="0" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="0" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="0" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="0" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="0" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A145" s="0" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A146" s="0" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="0" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A148" s="0" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A149" s="0" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="0" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="0" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A152" s="0" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="0" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A154" s="0" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A155" s="0" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A156" s="0" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="0" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="0" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A159" s="0" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="0" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A161" s="0" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="0" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A163" s="0" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="0" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="0" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A166" s="0" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="0" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="0" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="0" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="0" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="0" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A172" s="0" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A173" s="0" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="0" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="0" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="0" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="0" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="0" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="0" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="0" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="0" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="0" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="0" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="0" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A186" s="0" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="0" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="0" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="0" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="0" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="0" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="0" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A193" s="0" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A194" s="0" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A195" s="0" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="C196" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="F196" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="G196" s="0" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A197" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="C197" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="F197" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="G197" s="0" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A198" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="B198" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C198" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F198" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="G198" s="0" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="C199" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="F199" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="G199" s="0" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A200" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="C200" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="F200" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="G200" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="I200" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A201" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="C201" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="F201" s="0" t="s">
+        <v>279</v>
+      </c>
+      <c r="G201" s="0" t="s">
+        <v>280</v>
+      </c>
+      <c r="I201" s="0" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="0" t="s">
+        <v>282</v>
+      </c>
+      <c r="C202" s="0" t="s">
+        <v>283</v>
+      </c>
+      <c r="F202" s="0" t="s">
+        <v>284</v>
+      </c>
+      <c r="G202" s="0" t="s">
+        <v>285</v>
+      </c>
+      <c r="I202" s="0" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="0" t="s">
+        <v>287</v>
+      </c>
+      <c r="C203" s="0" t="s">
+        <v>288</v>
+      </c>
+      <c r="F203" s="0" t="s">
+        <v>289</v>
+      </c>
+      <c r="G203" s="0" t="s">
+        <v>290</v>
+      </c>
+      <c r="H203" s="0" t="s">
+        <v>291</v>
+      </c>
+      <c r="I203" s="0" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="0" t="s">
+        <v>293</v>
+      </c>
+      <c r="C204" s="0" t="s">
+        <v>294</v>
+      </c>
+      <c r="D204" s="0" t="s">
+        <v>295</v>
+      </c>
+      <c r="E204" s="0" t="s">
+        <v>296</v>
+      </c>
+      <c r="F204" s="0" t="s">
+        <v>297</v>
+      </c>
+      <c r="G204" s="0" t="s">
+        <v>298</v>
+      </c>
+      <c r="H204" s="0" t="s">
+        <v>299</v>
+      </c>
+      <c r="I204" s="0" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="0" t="s">
+        <v>301</v>
+      </c>
+      <c r="C205" s="0" t="s">
+        <v>302</v>
+      </c>
+      <c r="D205" s="0" t="s">
+        <v>303</v>
+      </c>
+      <c r="E205" s="0" t="s">
+        <v>304</v>
+      </c>
+      <c r="F205" s="0" t="s">
+        <v>305</v>
+      </c>
+      <c r="G205" s="0" t="s">
+        <v>306</v>
+      </c>
+      <c r="H205" s="0" t="s">
+        <v>307</v>
+      </c>
+      <c r="I205" s="0" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A206" s="0" t="s">
+        <v>309</v>
+      </c>
+      <c r="C206" s="0" t="s">
+        <v>310</v>
+      </c>
+      <c r="D206" s="0" t="s">
+        <v>311</v>
+      </c>
+      <c r="E206" s="0" t="s">
+        <v>312</v>
+      </c>
+      <c r="F206" s="0" t="s">
+        <v>313</v>
+      </c>
+      <c r="G206" s="0" t="s">
+        <v>314</v>
+      </c>
+      <c r="H206" s="0" t="s">
+        <v>315</v>
+      </c>
+      <c r="I206" s="0" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A207" s="0" t="s">
+        <v>317</v>
+      </c>
+      <c r="C207" s="0" t="s">
+        <v>318</v>
+      </c>
+      <c r="D207" s="0" t="s">
+        <v>319</v>
+      </c>
+      <c r="E207" s="0" t="s">
+        <v>320</v>
+      </c>
+      <c r="F207" s="0" t="s">
+        <v>321</v>
+      </c>
+      <c r="G207" s="0" t="s">
+        <v>322</v>
+      </c>
+      <c r="H207" s="0" t="s">
+        <v>323</v>
+      </c>
+      <c r="I207" s="0" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A208" s="0" t="s">
+        <v>325</v>
+      </c>
+      <c r="C208" s="0" t="s">
+        <v>326</v>
+      </c>
+      <c r="D208" s="0" t="s">
+        <v>327</v>
+      </c>
+      <c r="E208" s="0" t="s">
+        <v>328</v>
+      </c>
+      <c r="F208" s="0" t="s">
+        <v>329</v>
+      </c>
+      <c r="G208" s="0" t="s">
+        <v>330</v>
+      </c>
+      <c r="H208" s="0" t="s">
+        <v>331</v>
+      </c>
+      <c r="I208" s="0" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A209" s="0" t="s">
+        <v>333</v>
+      </c>
+      <c r="C209" s="0" t="s">
+        <v>334</v>
+      </c>
+      <c r="D209" s="0" t="s">
+        <v>335</v>
+      </c>
+      <c r="E209" s="0" t="s">
+        <v>336</v>
+      </c>
+      <c r="F209" s="0" t="s">
+        <v>337</v>
+      </c>
+      <c r="G209" s="0" t="s">
+        <v>338</v>
+      </c>
+      <c r="H209" s="0" t="s">
+        <v>339</v>
+      </c>
+      <c r="I209" s="0" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A210" s="0" t="s">
+        <v>341</v>
+      </c>
+      <c r="C210" s="0" t="s">
+        <v>342</v>
+      </c>
+      <c r="D210" s="0" t="s">
+        <v>343</v>
+      </c>
+      <c r="E210" s="0" t="s">
+        <v>344</v>
+      </c>
+      <c r="F210" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="G210" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="H210" s="0" t="s">
+        <v>347</v>
+      </c>
+      <c r="I210" s="0" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A211" s="0" t="s">
+        <v>349</v>
+      </c>
+      <c r="C211" s="0" t="s">
+        <v>350</v>
+      </c>
+      <c r="D211" s="0" t="s">
+        <v>351</v>
+      </c>
+      <c r="E211" s="0" t="s">
+        <v>352</v>
+      </c>
+      <c r="F211" s="0" t="s">
+        <v>353</v>
+      </c>
+      <c r="G211" s="0" t="s">
+        <v>354</v>
+      </c>
+      <c r="H211" s="0" t="s">
+        <v>355</v>
+      </c>
+      <c r="I211" s="0" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A212" s="4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>

<commit_message>
Continuar posición patrones sprites
Se corrige la posición de memoria de patrones
Se define posiciones para la fase 0,1 y 2
</commit_message>
<xml_diff>
--- a/doc/análisis posición en memoria sprites enemigos.xlsx
+++ b/doc/análisis posición en memoria sprites enemigos.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="185">
   <si>
     <t xml:space="preserve">Nombre Enemigo</t>
   </si>
@@ -197,604 +197,133 @@
     <t xml:space="preserve">Sprites comunes</t>
   </si>
   <si>
-    <t xml:space="preserve">3800h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_punto_mira_1</t>
   </si>
   <si>
-    <t xml:space="preserve">3820h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_punto_mira_2</t>
   </si>
   <si>
-    <t xml:space="preserve">3840h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_punto_mira_1_mejorado</t>
   </si>
   <si>
-    <t xml:space="preserve">3860h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_punto_mira_2_mejorado</t>
   </si>
   <si>
-    <t xml:space="preserve">3880h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_explosion</t>
   </si>
   <si>
-    <t xml:space="preserve">3900h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3920h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3940h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3960h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3980h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4000h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4020h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4040h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4060h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4080h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4100h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4120h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4140h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4160h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4180h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4200h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4220h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4240h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4260h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4280h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4300h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4320h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4340h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4360h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4380h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4400h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4420h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4440h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4460h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4480h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4500h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4520h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4540h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4560h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4580h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4600h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4620h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4640h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4660h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4680h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4700h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4720h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4740h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4760h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4780h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4800h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4820h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4840h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4860h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4880h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4900h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4920h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4940h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4960h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4980h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5000h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5020h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5040h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5060h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5080h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5100h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5120h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5140h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5160h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5180h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5200h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5220h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5240h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5260h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5280h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5300h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5320h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5340h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5360h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5380h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5400h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5420h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5440h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5460h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5480h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5500h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5520h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5540h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5560h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5580h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5600h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5620h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5640h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5660h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5680h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5700h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5720h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5740h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5760h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5780h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5800h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5820h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5840h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5860h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5880h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5900h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5920h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5940h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5960h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5980h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6000h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6020h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6040h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6060h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6080h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6100h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6120h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6140h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6160h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6180h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6200h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6220h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6240h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6260h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6280h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6300h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6320h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6340h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6360h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6380h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6400h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6420h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6440h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6460h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6480h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6500h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6520h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6540h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6560h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6580h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6600h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6620h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6640h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6660h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6680h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6700h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6720h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6740h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6760h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6780h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6800h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6820h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6840h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6860h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6880h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6900h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6920h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6940h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6960h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">6980h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7000h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7020h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7040h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7060h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7080h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7100h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7120h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7140h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7160h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7180h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7200h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7220h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7240h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7260h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7280h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7300h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7320h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7340h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7360h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7380h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7400h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7420h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7440h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7460h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7480h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7500h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7520h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7540h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7560h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7580h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7600h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7620h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7640h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7660h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7680h</t>
+    <t xml:space="preserve">sprite_cienpies_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_cienpies_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_serpiente1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_serpiente1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_serpiente2_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_serpiente2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_arana_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_arana_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_murcielago_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_murcielago_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_lobo1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_lobo1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_lobo1_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_lobo1_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_lobo2_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_lobo2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_lobo2_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_lobo2_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_esqueleto1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_esqueleto1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_esqueleto1_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_esqueleto1_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_esqueleto2_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_esqueleto2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_esqueleto2_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_esqueleto2_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_zombi1_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_zombi1_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_zombi1_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_zombi1_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_zombi2_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_zombi2_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_zombi2_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_zombi2_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_fantasma_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_fantasma_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_fantasma_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_fantasma_4</t>
   </si>
   <si>
     <t xml:space="preserve">sprite_jefelobo1_1</t>
@@ -806,9 +335,6 @@
     <t xml:space="preserve">sprite_jefecaballero1_1</t>
   </si>
   <si>
-    <t xml:space="preserve">7700h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo1_2</t>
   </si>
   <si>
@@ -818,9 +344,6 @@
     <t xml:space="preserve">sprite_jefecaballero1_2</t>
   </si>
   <si>
-    <t xml:space="preserve">7720h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo1_3</t>
   </si>
   <si>
@@ -830,9 +353,6 @@
     <t xml:space="preserve">sprite_jefecaballero1_3</t>
   </si>
   <si>
-    <t xml:space="preserve">7740h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo1_4</t>
   </si>
   <si>
@@ -842,9 +362,6 @@
     <t xml:space="preserve">sprite_jefecaballero1_4</t>
   </si>
   <si>
-    <t xml:space="preserve">7760h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo1_5</t>
   </si>
   <si>
@@ -857,9 +374,6 @@
     <t xml:space="preserve">sprite_manoizquierda_1</t>
   </si>
   <si>
-    <t xml:space="preserve">7780h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo1_6</t>
   </si>
   <si>
@@ -872,9 +386,6 @@
     <t xml:space="preserve">sprite_manoizquierda_2</t>
   </si>
   <si>
-    <t xml:space="preserve">7800h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo1_7</t>
   </si>
   <si>
@@ -887,9 +398,6 @@
     <t xml:space="preserve">sprite_manoizquierda_3</t>
   </si>
   <si>
-    <t xml:space="preserve">7820h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo1_8</t>
   </si>
   <si>
@@ -905,9 +413,6 @@
     <t xml:space="preserve">sprite_manoizquierda_4</t>
   </si>
   <si>
-    <t xml:space="preserve">7840h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo2_1</t>
   </si>
   <si>
@@ -929,9 +434,6 @@
     <t xml:space="preserve">sprite_manoderecha_1</t>
   </si>
   <si>
-    <t xml:space="preserve">7860h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo2_2</t>
   </si>
   <si>
@@ -953,9 +455,6 @@
     <t xml:space="preserve">sprite_manoderecha_2</t>
   </si>
   <si>
-    <t xml:space="preserve">7880h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo2_3</t>
   </si>
   <si>
@@ -977,9 +476,6 @@
     <t xml:space="preserve">sprite_manoderecha_3</t>
   </si>
   <si>
-    <t xml:space="preserve">7900h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo2_4</t>
   </si>
   <si>
@@ -1001,9 +497,6 @@
     <t xml:space="preserve">sprite_manoderecha_4</t>
   </si>
   <si>
-    <t xml:space="preserve">7920h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo2_5</t>
   </si>
   <si>
@@ -1025,9 +518,6 @@
     <t xml:space="preserve">sprite_conde_1</t>
   </si>
   <si>
-    <t xml:space="preserve">7940h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo2_6</t>
   </si>
   <si>
@@ -1049,9 +539,6 @@
     <t xml:space="preserve">sprite_conde_2</t>
   </si>
   <si>
-    <t xml:space="preserve">7960h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo2_7</t>
   </si>
   <si>
@@ -1073,9 +560,6 @@
     <t xml:space="preserve">sprite_conde_3</t>
   </si>
   <si>
-    <t xml:space="preserve">7980h</t>
-  </si>
-  <si>
     <t xml:space="preserve">sprite_jefelobo2_8</t>
   </si>
   <si>
@@ -1095,17 +579,15 @@
   </si>
   <si>
     <t xml:space="preserve">sprite_conde_4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">8000h</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -1185,7 +667,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1198,7 +680,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1226,10 +716,10 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N5" activeCellId="0" sqref="N5"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="1" sqref="F9:F12 H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.07"/>
@@ -1922,10 +1412,10 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="1" sqref="F9:F12 B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2089,10 +1579,10 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="1" sqref="F9:F12 B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.65"/>
   </cols>
@@ -2292,30 +1782,30 @@
   <dimension ref="A1:AA65"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y1" activeCellId="0" sqref="Y1"/>
+      <selection pane="topLeft" activeCell="Y1" activeCellId="1" sqref="F9:F12 Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="2.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="2.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="2.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="2.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="2.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="2.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="2.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="2.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="2.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="2.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="2.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="10.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="2.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="2.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="2.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="10.92"/>
   </cols>
@@ -4080,1417 +3570,1808 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I212"/>
+  <dimension ref="A1:O212"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9:F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="26.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="B1" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="E1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="F1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="G1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="H1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="I1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="J1" s="0" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="0" t="n">
+        <v>14336</v>
+      </c>
+      <c r="B2" s="0" t="str">
+        <f aca="false">DEC2HEX(A2)</f>
+        <v>3800</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>14368</v>
+      </c>
+      <c r="B3" s="0" t="str">
+        <f aca="false">DEC2HEX(A3)</f>
+        <v>3820</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>14400</v>
+      </c>
+      <c r="B4" s="0" t="str">
+        <f aca="false">DEC2HEX(A4)</f>
+        <v>3840</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>14432</v>
+      </c>
+      <c r="B5" s="0" t="str">
+        <f aca="false">DEC2HEX(A5)</f>
+        <v>3860</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>14464</v>
+      </c>
+      <c r="B6" s="0" t="str">
+        <f aca="false">DEC2HEX(A6)</f>
+        <v>3880</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>14496</v>
+      </c>
+      <c r="B7" s="0" t="str">
+        <f aca="false">DEC2HEX(A7)</f>
+        <v>38A0</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>14528</v>
+      </c>
+      <c r="B8" s="0" t="str">
+        <f aca="false">DEC2HEX(A8)</f>
+        <v>38C0</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>14560</v>
+      </c>
+      <c r="B9" s="0" t="str">
+        <f aca="false">DEC2HEX(A9)</f>
+        <v>38E0</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="E9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>14592</v>
+      </c>
+      <c r="B10" s="0" t="str">
+        <f aca="false">DEC2HEX(A10)</f>
+        <v>3900</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="E10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>14624</v>
+      </c>
+      <c r="B11" s="0" t="str">
+        <f aca="false">DEC2HEX(A11)</f>
+        <v>3920</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="E11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>14656</v>
+      </c>
+      <c r="B12" s="0" t="str">
+        <f aca="false">DEC2HEX(A12)</f>
+        <v>3940</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="E12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+      <c r="M12" s="5"/>
+      <c r="N12" s="5"/>
+      <c r="O12" s="5"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>14688</v>
+      </c>
+      <c r="B13" s="0" t="str">
+        <f aca="false">DEC2HEX(A13)</f>
+        <v>3960</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="E13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5"/>
+      <c r="M13" s="5"/>
+      <c r="N13" s="5"/>
+      <c r="O13" s="5"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>14720</v>
+      </c>
+      <c r="B14" s="0" t="str">
+        <f aca="false">DEC2HEX(A14)</f>
+        <v>3980</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="E14" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5"/>
+      <c r="M14" s="5"/>
+      <c r="N14" s="5"/>
+      <c r="O14" s="5"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14752</v>
+      </c>
+      <c r="B15" s="0" t="str">
+        <f aca="false">DEC2HEX(A15)</f>
+        <v>39A0</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="E15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>14784</v>
+      </c>
+      <c r="B16" s="0" t="str">
+        <f aca="false">DEC2HEX(A16)</f>
+        <v>39C0</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="E16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+      <c r="O16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>14816</v>
+      </c>
+      <c r="B17" s="0" t="str">
+        <f aca="false">DEC2HEX(A17)</f>
+        <v>39E0</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="E17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>14848</v>
+      </c>
+      <c r="B18" s="0" t="str">
+        <f aca="false">DEC2HEX(A18)</f>
+        <v>3A00</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="E18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>14880</v>
+      </c>
+      <c r="B19" s="0" t="str">
+        <f aca="false">DEC2HEX(A19)</f>
+        <v>3A20</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="E19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5"/>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>14912</v>
+      </c>
+      <c r="B20" s="0" t="str">
+        <f aca="false">DEC2HEX(A20)</f>
+        <v>3A40</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="E20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>14944</v>
+      </c>
+      <c r="B21" s="0" t="str">
+        <f aca="false">DEC2HEX(A21)</f>
+        <v>3A60</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="E21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>14976</v>
+      </c>
+      <c r="B22" s="0" t="str">
+        <f aca="false">DEC2HEX(A22)</f>
+        <v>3A80</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="E22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>15008</v>
+      </c>
+      <c r="B23" s="0" t="str">
+        <f aca="false">DEC2HEX(A23)</f>
+        <v>3AA0</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="E23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5"/>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>15040</v>
+      </c>
+      <c r="B24" s="0" t="str">
+        <f aca="false">DEC2HEX(A24)</f>
+        <v>3AC0</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="E24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5"/>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>15072</v>
+      </c>
+      <c r="B25" s="0" t="str">
+        <f aca="false">DEC2HEX(A25)</f>
+        <v>3AE0</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="F25" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5"/>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>15104</v>
+      </c>
+      <c r="B26" s="0" t="str">
+        <f aca="false">DEC2HEX(A26)</f>
+        <v>3B00</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="F26" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5"/>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>15136</v>
+      </c>
+      <c r="B27" s="0" t="str">
+        <f aca="false">DEC2HEX(A27)</f>
+        <v>3B20</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="F27" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>15168</v>
+      </c>
+      <c r="B28" s="0" t="str">
+        <f aca="false">DEC2HEX(A28)</f>
+        <v>3B40</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="F28" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5"/>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>15200</v>
+      </c>
+      <c r="B29" s="0" t="str">
+        <f aca="false">DEC2HEX(A29)</f>
+        <v>3B60</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="F29" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5"/>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>15232</v>
+      </c>
+      <c r="B30" s="0" t="str">
+        <f aca="false">DEC2HEX(A30)</f>
+        <v>3B80</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="F30" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5"/>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>15264</v>
+      </c>
+      <c r="B31" s="0" t="str">
+        <f aca="false">DEC2HEX(A31)</f>
+        <v>3BA0</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="F31" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5"/>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>15296</v>
+      </c>
+      <c r="B32" s="0" t="str">
+        <f aca="false">DEC2HEX(A32)</f>
+        <v>3BC0</v>
+      </c>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="F32" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5"/>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>15328</v>
+      </c>
+      <c r="B33" s="0" t="str">
+        <f aca="false">DEC2HEX(A33)</f>
+        <v>3BE0</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="F33" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>15360</v>
+      </c>
+      <c r="B34" s="0" t="str">
+        <f aca="false">DEC2HEX(A34)</f>
+        <v>3C00</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="F34" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5"/>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>15392</v>
+      </c>
+      <c r="B35" s="0" t="str">
+        <f aca="false">DEC2HEX(A35)</f>
+        <v>3C20</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="F35" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>15424</v>
+      </c>
+      <c r="B36" s="0" t="str">
+        <f aca="false">DEC2HEX(A36)</f>
+        <v>3C40</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="F36" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="5"/>
+      <c r="N36" s="5"/>
+      <c r="O36" s="5"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>15456</v>
+      </c>
+      <c r="B37" s="0" t="str">
+        <f aca="false">DEC2HEX(A37)</f>
+        <v>3C60</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="F37" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5"/>
+      <c r="M37" s="5"/>
+      <c r="N37" s="5"/>
+      <c r="O37" s="5"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>15488</v>
+      </c>
+      <c r="B38" s="0" t="str">
+        <f aca="false">DEC2HEX(A38)</f>
+        <v>3C80</v>
+      </c>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="F38" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G38" s="3"/>
+      <c r="H38" s="3"/>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5"/>
+      <c r="M38" s="5"/>
+      <c r="N38" s="5"/>
+      <c r="O38" s="5"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>15520</v>
+      </c>
+      <c r="B39" s="0" t="str">
+        <f aca="false">DEC2HEX(A39)</f>
+        <v>3CA0</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+      <c r="E39" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="F39" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="5"/>
+      <c r="N39" s="5"/>
+      <c r="O39" s="5"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>15552</v>
+      </c>
+      <c r="B40" s="0" t="str">
+        <f aca="false">DEC2HEX(A40)</f>
+        <v>3CC0</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="F40" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5"/>
+      <c r="M40" s="5"/>
+      <c r="N40" s="5"/>
+      <c r="O40" s="5"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>15584</v>
+      </c>
+      <c r="B41" s="0" t="str">
+        <f aca="false">DEC2HEX(A41)</f>
+        <v>3CE0</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
+      <c r="F41" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5"/>
+      <c r="M41" s="5"/>
+      <c r="N41" s="5"/>
+      <c r="O41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>15616</v>
+      </c>
+      <c r="B42" s="0" t="str">
+        <f aca="false">DEC2HEX(A42)</f>
+        <v>3D00</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="F42" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5"/>
+      <c r="M42" s="5"/>
+      <c r="N42" s="5"/>
+      <c r="O42" s="5"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>15648</v>
+      </c>
+      <c r="B43" s="0" t="str">
+        <f aca="false">DEC2HEX(A43)</f>
+        <v>3D20</v>
+      </c>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="F43" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5"/>
+      <c r="M43" s="5"/>
+      <c r="N43" s="5"/>
+      <c r="O43" s="5"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>15680</v>
+      </c>
+      <c r="B44" s="0" t="str">
+        <f aca="false">DEC2HEX(A44)</f>
+        <v>3D40</v>
+      </c>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="F44" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>15712</v>
+      </c>
+      <c r="B45" s="0" t="str">
+        <f aca="false">DEC2HEX(A45)</f>
+        <v>3D60</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>15744</v>
+      </c>
+      <c r="B46" s="0" t="str">
+        <f aca="false">DEC2HEX(A46)</f>
+        <v>3D80</v>
+      </c>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>15776</v>
+      </c>
+      <c r="B47" s="0" t="str">
+        <f aca="false">DEC2HEX(A47)</f>
+        <v>3DA0</v>
+      </c>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5"/>
+      <c r="M47" s="5"/>
+      <c r="N47" s="5"/>
+      <c r="O47" s="5"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>15808</v>
+      </c>
+      <c r="B48" s="0" t="str">
+        <f aca="false">DEC2HEX(A48)</f>
+        <v>3DC0</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5"/>
+      <c r="M48" s="5"/>
+      <c r="N48" s="5"/>
+      <c r="O48" s="5"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>15840</v>
+      </c>
+      <c r="B49" s="0" t="str">
+        <f aca="false">DEC2HEX(A49)</f>
+        <v>3DE0</v>
+      </c>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="5"/>
+      <c r="L49" s="5"/>
+      <c r="M49" s="5"/>
+      <c r="N49" s="5"/>
+      <c r="O49" s="5"/>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>15872</v>
+      </c>
+      <c r="B50" s="0" t="str">
+        <f aca="false">DEC2HEX(A50)</f>
+        <v>3E00</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="H50" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="5"/>
+      <c r="L50" s="5"/>
+      <c r="M50" s="5"/>
+      <c r="N50" s="5"/>
+      <c r="O50" s="5"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>15904</v>
+      </c>
+      <c r="B51" s="0" t="str">
+        <f aca="false">DEC2HEX(A51)</f>
+        <v>3E20</v>
+      </c>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="H51" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5"/>
+      <c r="O51" s="5"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>15936</v>
+      </c>
+      <c r="B52" s="0" t="str">
+        <f aca="false">DEC2HEX(A52)</f>
+        <v>3E40</v>
+      </c>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="E52" s="3"/>
+      <c r="F52" s="3"/>
+      <c r="G52" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="H52" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="5"/>
+      <c r="L52" s="5"/>
+      <c r="M52" s="5"/>
+      <c r="N52" s="5"/>
+      <c r="O52" s="5"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>15968</v>
+      </c>
+      <c r="B53" s="0" t="str">
+        <f aca="false">DEC2HEX(A53)</f>
+        <v>3E60</v>
+      </c>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="H53" s="3" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="5"/>
+      <c r="L53" s="5"/>
+      <c r="M53" s="5"/>
+      <c r="N53" s="5"/>
+      <c r="O53" s="5"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>16000</v>
+      </c>
+      <c r="B54" s="0" t="str">
+        <f aca="false">DEC2HEX(A54)</f>
+        <v>3E80</v>
+      </c>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="H54" s="3" t="s">
         <v>114</v>
       </c>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="K54" s="5"/>
+      <c r="L54" s="5"/>
+      <c r="M54" s="5"/>
+      <c r="N54" s="5"/>
+      <c r="O54" s="5"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
-        <v>115</v>
-      </c>
+      <c r="A55" s="0" t="n">
+        <v>16032</v>
+      </c>
+      <c r="B55" s="0" t="str">
+        <f aca="false">DEC2HEX(A55)</f>
+        <v>3EA0</v>
+      </c>
+      <c r="C55" s="3"/>
+      <c r="D55" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="K55" s="5"/>
+      <c r="L55" s="5"/>
+      <c r="M55" s="5"/>
+      <c r="N55" s="5"/>
+      <c r="O55" s="5"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
-        <v>116</v>
-      </c>
+      <c r="A56" s="0" t="n">
+        <v>16064</v>
+      </c>
+      <c r="B56" s="0" t="str">
+        <f aca="false">DEC2HEX(A56)</f>
+        <v>3EC0</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="K56" s="5"/>
+      <c r="L56" s="5"/>
+      <c r="M56" s="5"/>
+      <c r="N56" s="5"/>
+      <c r="O56" s="5"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
-        <v>117</v>
-      </c>
+      <c r="A57" s="0" t="n">
+        <v>16096</v>
+      </c>
+      <c r="B57" s="0" t="str">
+        <f aca="false">DEC2HEX(A57)</f>
+        <v>3EE0</v>
+      </c>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
+      <c r="G57" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="K57" s="5"/>
+      <c r="L57" s="5"/>
+      <c r="M57" s="5"/>
+      <c r="N57" s="5"/>
+      <c r="O57" s="5"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>118</v>
-      </c>
+      <c r="A58" s="0" t="n">
+        <v>16128</v>
+      </c>
+      <c r="B58" s="0" t="str">
+        <f aca="false">DEC2HEX(A58)</f>
+        <v>3F00</v>
+      </c>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="K58" s="5"/>
+      <c r="L58" s="5"/>
+      <c r="M58" s="5"/>
+      <c r="N58" s="5"/>
+      <c r="O58" s="5"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
-        <v>119</v>
-      </c>
+      <c r="A59" s="0" t="n">
+        <v>16160</v>
+      </c>
+      <c r="B59" s="0" t="str">
+        <f aca="false">DEC2HEX(A59)</f>
+        <v>3F20</v>
+      </c>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="5"/>
+      <c r="N59" s="5"/>
+      <c r="O59" s="5"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
-        <v>120</v>
-      </c>
+      <c r="A60" s="0" t="n">
+        <v>16192</v>
+      </c>
+      <c r="B60" s="0" t="str">
+        <f aca="false">DEC2HEX(A60)</f>
+        <v>3F40</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="K60" s="5"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="5"/>
+      <c r="N60" s="5"/>
+      <c r="O60" s="5"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
-        <v>121</v>
-      </c>
+      <c r="A61" s="0" t="n">
+        <v>16224</v>
+      </c>
+      <c r="B61" s="0" t="str">
+        <f aca="false">DEC2HEX(A61)</f>
+        <v>3F60</v>
+      </c>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="5"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
-        <v>122</v>
-      </c>
+      <c r="A62" s="0" t="n">
+        <v>16256</v>
+      </c>
+      <c r="B62" s="0" t="str">
+        <f aca="false">DEC2HEX(A62)</f>
+        <v>3F80</v>
+      </c>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="5"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
-        <v>123</v>
-      </c>
+      <c r="A63" s="0" t="n">
+        <v>16288</v>
+      </c>
+      <c r="B63" s="0" t="str">
+        <f aca="false">DEC2HEX(A63)</f>
+        <v>3FA0</v>
+      </c>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="K63" s="5"/>
+      <c r="L63" s="5"/>
+      <c r="M63" s="5"/>
+      <c r="N63" s="5"/>
+      <c r="O63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
-        <v>124</v>
-      </c>
+      <c r="A64" s="0" t="n">
+        <v>16320</v>
+      </c>
+      <c r="B64" s="0" t="str">
+        <f aca="false">DEC2HEX(A64)</f>
+        <v>3FC0</v>
+      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="K64" s="5"/>
+      <c r="L64" s="5"/>
+      <c r="M64" s="5"/>
+      <c r="N64" s="5"/>
+      <c r="O64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="0" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="0" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="0" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="0" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="0" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="0" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="0" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="0" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="0" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="0" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="0" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="0" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="0" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="0" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="0" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="0" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="0" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="0" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="0" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="0" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="0" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="0" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="0" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="0" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="0" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="0" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="0" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="0" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="0" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="0" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="0" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="0" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="0" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="0" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="0" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="0" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="0" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="0" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="0" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="0" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="0" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="0" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="0" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="0" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="0" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="0" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="0" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="0" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="0" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="0" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="0" t="s">
+      <c r="A65" s="0" t="n">
+        <v>16352</v>
+      </c>
+      <c r="B65" s="0" t="str">
+        <f aca="false">DEC2HEX(A65)</f>
+        <v>3FE0</v>
+      </c>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="0" t="s">
+      <c r="E65" s="3" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="0" t="s">
+      <c r="F65" s="3" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="0" t="s">
+      <c r="G65" s="3" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="0" t="s">
+      <c r="H65" s="3" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="0" t="s">
+      <c r="I65" s="3" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="0" t="s">
+      <c r="J65" s="3" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="0" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="0" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="0" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="0" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="0" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="0" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="0" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="0" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="0" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="0" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="0" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="0" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="0" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="0" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="0" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="0" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="0" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="0" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="0" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="0" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A145" s="0" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A146" s="0" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="0" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="0" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A149" s="0" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="0" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="0" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A152" s="0" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="0" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A154" s="0" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A155" s="0" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="0" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="0" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="0" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="0" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="0" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A161" s="0" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="0" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A163" s="0" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="0" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="0" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A166" s="0" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="0" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="0" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="0" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="0" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="0" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A172" s="0" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A173" s="0" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="0" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="0" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="0" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="0" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="0" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="0" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="0" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="0" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="0" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="0" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="0" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="0" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A186" s="0" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="0" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A188" s="0" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A189" s="0" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A190" s="0" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A191" s="0" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A192" s="0" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A193" s="0" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="0" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A195" s="0" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="0" t="s">
-        <v>256</v>
-      </c>
-      <c r="C196" s="0" t="s">
-        <v>257</v>
-      </c>
-      <c r="F196" s="0" t="s">
-        <v>258</v>
-      </c>
-      <c r="G196" s="0" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A197" s="0" t="s">
-        <v>260</v>
-      </c>
-      <c r="C197" s="0" t="s">
-        <v>261</v>
-      </c>
-      <c r="F197" s="0" t="s">
-        <v>262</v>
-      </c>
-      <c r="G197" s="0" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="0" t="s">
-        <v>264</v>
-      </c>
-      <c r="B198" s="0" t="n">
-        <v>9</v>
-      </c>
-      <c r="C198" s="0" t="s">
-        <v>265</v>
-      </c>
-      <c r="F198" s="0" t="s">
-        <v>266</v>
-      </c>
-      <c r="G198" s="0" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="0" t="s">
-        <v>268</v>
-      </c>
-      <c r="C199" s="0" t="s">
-        <v>269</v>
-      </c>
-      <c r="F199" s="0" t="s">
-        <v>270</v>
-      </c>
-      <c r="G199" s="0" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="0" t="s">
-        <v>272</v>
-      </c>
-      <c r="C200" s="0" t="s">
-        <v>273</v>
-      </c>
-      <c r="F200" s="0" t="s">
-        <v>274</v>
-      </c>
-      <c r="G200" s="0" t="s">
-        <v>275</v>
-      </c>
-      <c r="I200" s="0" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="0" t="s">
-        <v>277</v>
-      </c>
-      <c r="C201" s="0" t="s">
-        <v>278</v>
-      </c>
-      <c r="F201" s="0" t="s">
-        <v>279</v>
-      </c>
-      <c r="G201" s="0" t="s">
-        <v>280</v>
-      </c>
-      <c r="I201" s="0" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="0" t="s">
-        <v>282</v>
-      </c>
-      <c r="C202" s="0" t="s">
-        <v>283</v>
-      </c>
-      <c r="F202" s="0" t="s">
-        <v>284</v>
-      </c>
-      <c r="G202" s="0" t="s">
-        <v>285</v>
-      </c>
-      <c r="I202" s="0" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="0" t="s">
-        <v>287</v>
-      </c>
-      <c r="C203" s="0" t="s">
-        <v>288</v>
-      </c>
-      <c r="F203" s="0" t="s">
-        <v>289</v>
-      </c>
-      <c r="G203" s="0" t="s">
-        <v>290</v>
-      </c>
-      <c r="H203" s="0" t="s">
-        <v>291</v>
-      </c>
-      <c r="I203" s="0" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A204" s="0" t="s">
-        <v>293</v>
-      </c>
-      <c r="C204" s="0" t="s">
-        <v>294</v>
-      </c>
-      <c r="D204" s="0" t="s">
-        <v>295</v>
-      </c>
-      <c r="E204" s="0" t="s">
-        <v>296</v>
-      </c>
-      <c r="F204" s="0" t="s">
-        <v>297</v>
-      </c>
-      <c r="G204" s="0" t="s">
-        <v>298</v>
-      </c>
-      <c r="H204" s="0" t="s">
-        <v>299</v>
-      </c>
-      <c r="I204" s="0" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A205" s="0" t="s">
-        <v>301</v>
-      </c>
-      <c r="C205" s="0" t="s">
-        <v>302</v>
-      </c>
-      <c r="D205" s="0" t="s">
-        <v>303</v>
-      </c>
-      <c r="E205" s="0" t="s">
-        <v>304</v>
-      </c>
-      <c r="F205" s="0" t="s">
-        <v>305</v>
-      </c>
-      <c r="G205" s="0" t="s">
-        <v>306</v>
-      </c>
-      <c r="H205" s="0" t="s">
-        <v>307</v>
-      </c>
-      <c r="I205" s="0" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A206" s="0" t="s">
-        <v>309</v>
-      </c>
-      <c r="C206" s="0" t="s">
-        <v>310</v>
-      </c>
-      <c r="D206" s="0" t="s">
-        <v>311</v>
-      </c>
-      <c r="E206" s="0" t="s">
-        <v>312</v>
-      </c>
-      <c r="F206" s="0" t="s">
-        <v>313</v>
-      </c>
-      <c r="G206" s="0" t="s">
-        <v>314</v>
-      </c>
-      <c r="H206" s="0" t="s">
-        <v>315</v>
-      </c>
-      <c r="I206" s="0" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A207" s="0" t="s">
-        <v>317</v>
-      </c>
-      <c r="C207" s="0" t="s">
-        <v>318</v>
-      </c>
-      <c r="D207" s="0" t="s">
-        <v>319</v>
-      </c>
-      <c r="E207" s="0" t="s">
-        <v>320</v>
-      </c>
-      <c r="F207" s="0" t="s">
-        <v>321</v>
-      </c>
-      <c r="G207" s="0" t="s">
-        <v>322</v>
-      </c>
-      <c r="H207" s="0" t="s">
-        <v>323</v>
-      </c>
-      <c r="I207" s="0" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A208" s="0" t="s">
-        <v>325</v>
-      </c>
-      <c r="C208" s="0" t="s">
-        <v>326</v>
-      </c>
-      <c r="D208" s="0" t="s">
-        <v>327</v>
-      </c>
-      <c r="E208" s="0" t="s">
-        <v>328</v>
-      </c>
-      <c r="F208" s="0" t="s">
-        <v>329</v>
-      </c>
-      <c r="G208" s="0" t="s">
-        <v>330</v>
-      </c>
-      <c r="H208" s="0" t="s">
-        <v>331</v>
-      </c>
-      <c r="I208" s="0" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A209" s="0" t="s">
-        <v>333</v>
-      </c>
-      <c r="C209" s="0" t="s">
-        <v>334</v>
-      </c>
-      <c r="D209" s="0" t="s">
-        <v>335</v>
-      </c>
-      <c r="E209" s="0" t="s">
-        <v>336</v>
-      </c>
-      <c r="F209" s="0" t="s">
-        <v>337</v>
-      </c>
-      <c r="G209" s="0" t="s">
-        <v>338</v>
-      </c>
-      <c r="H209" s="0" t="s">
-        <v>339</v>
-      </c>
-      <c r="I209" s="0" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A210" s="0" t="s">
-        <v>341</v>
-      </c>
-      <c r="C210" s="0" t="s">
-        <v>342</v>
-      </c>
-      <c r="D210" s="0" t="s">
-        <v>343</v>
-      </c>
-      <c r="E210" s="0" t="s">
-        <v>344</v>
-      </c>
-      <c r="F210" s="0" t="s">
-        <v>345</v>
-      </c>
-      <c r="G210" s="0" t="s">
-        <v>346</v>
-      </c>
-      <c r="H210" s="0" t="s">
-        <v>347</v>
-      </c>
-      <c r="I210" s="0" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A211" s="0" t="s">
-        <v>349</v>
-      </c>
-      <c r="C211" s="0" t="s">
-        <v>350</v>
-      </c>
-      <c r="D211" s="0" t="s">
-        <v>351</v>
-      </c>
-      <c r="E211" s="0" t="s">
-        <v>352</v>
-      </c>
-      <c r="F211" s="0" t="s">
-        <v>353</v>
-      </c>
-      <c r="G211" s="0" t="s">
-        <v>354</v>
-      </c>
-      <c r="H211" s="0" t="s">
-        <v>355</v>
-      </c>
-      <c r="I211" s="0" t="s">
-        <v>356</v>
-      </c>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="5"/>
+      <c r="O65" s="5"/>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A212" s="4" t="s">
-        <v>357</v>
-      </c>
+      <c r="B212" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Continuación definir pos patrones sprites
Fin posiciones de memoria
Falta definir posiciones OAM
</commit_message>
<xml_diff>
--- a/doc/análisis posición en memoria sprites enemigos.xlsx
+++ b/doc/análisis posición en memoria sprites enemigos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="lista enemigos" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="202">
   <si>
     <t xml:space="preserve">Nombre Enemigo</t>
   </si>
@@ -191,7 +191,10 @@
     <t xml:space="preserve">explosión</t>
   </si>
   <si>
-    <t xml:space="preserve">Dirección memoria</t>
+    <t xml:space="preserve">Dirección Dec.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dirección Hex.</t>
   </si>
   <si>
     <t xml:space="preserve">Sprites comunes</t>
@@ -218,15 +221,27 @@
     <t xml:space="preserve">sprite_cienpies_2</t>
   </si>
   <si>
+    <t xml:space="preserve">sprite_magia_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">sprite_serpiente1_1</t>
   </si>
   <si>
+    <t xml:space="preserve">sprite_magia_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">sprite_serpiente1_2</t>
   </si>
   <si>
+    <t xml:space="preserve">sprite_magia_3</t>
+  </si>
+  <si>
     <t xml:space="preserve">sprite_serpiente2_1</t>
   </si>
   <si>
+    <t xml:space="preserve">sprite_magia_4</t>
+  </si>
+  <si>
     <t xml:space="preserve">sprite_serpiente2_2</t>
   </si>
   <si>
@@ -245,27 +260,51 @@
     <t xml:space="preserve">sprite_lobo1_1</t>
   </si>
   <si>
+    <t xml:space="preserve">sprite_caballero1_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">sprite_lobo1_2</t>
   </si>
   <si>
+    <t xml:space="preserve">sprite_caballero1_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">sprite_lobo1_3</t>
   </si>
   <si>
+    <t xml:space="preserve">sprite_caballero1_3</t>
+  </si>
+  <si>
     <t xml:space="preserve">sprite_lobo1_4</t>
   </si>
   <si>
+    <t xml:space="preserve">sprite_caballero1_4</t>
+  </si>
+  <si>
     <t xml:space="preserve">sprite_lobo2_1</t>
   </si>
   <si>
+    <t xml:space="preserve">sprite_caballero2_1</t>
+  </si>
+  <si>
     <t xml:space="preserve">sprite_lobo2_2</t>
   </si>
   <si>
+    <t xml:space="preserve">sprite_caballero2_2</t>
+  </si>
+  <si>
     <t xml:space="preserve">sprite_lobo2_3</t>
   </si>
   <si>
+    <t xml:space="preserve">sprite_caballero2_3</t>
+  </si>
+  <si>
     <t xml:space="preserve">sprite_lobo2_4</t>
   </si>
   <si>
+    <t xml:space="preserve">sprite_caballero2_4</t>
+  </si>
+  <si>
     <t xml:space="preserve">sprite_esqueleto1_1</t>
   </si>
   <si>
@@ -324,6 +363,18 @@
   </si>
   <si>
     <t xml:space="preserve">sprite_fantasma_4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_fuego_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_fuego_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_fuego_3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sprite_fuego_4</t>
   </si>
   <si>
     <t xml:space="preserve">sprite_jefelobo1_1</t>
@@ -619,7 +670,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -628,17 +679,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FF999999"/>
+        <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FF333333"/>
         <bgColor rgb="FF333300"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -667,7 +737,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -680,15 +750,27 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -705,6 +787,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF999999"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -716,10 +858,10 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="1" sqref="F9:F12 H5"/>
+      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.07"/>
@@ -822,7 +964,9 @@
       <c r="H3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -919,9 +1063,7 @@
       <c r="H6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
         <v>14</v>
@@ -1412,10 +1554,10 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="1" sqref="F9:F12 B13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1579,10 +1721,10 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="1" sqref="F9:F12 B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.65"/>
   </cols>
@@ -1779,18 +1921,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA65"/>
+  <dimension ref="A1:AA33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y1" activeCellId="1" sqref="F9:F12 Y1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="2.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="11.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="2.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="2.38"/>
@@ -2818,742 +2959,6 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="E34" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="I34" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="M34" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="Q34" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="U34" s="0" t="n">
-        <v>32</v>
-      </c>
-      <c r="Y34" s="0" t="n">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="E35" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="I35" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="M35" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="Q35" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="U35" s="0" t="n">
-        <v>33</v>
-      </c>
-      <c r="Y35" s="0" t="n">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="E36" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="I36" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="M36" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="Q36" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="U36" s="0" t="n">
-        <v>34</v>
-      </c>
-      <c r="Y36" s="0" t="n">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="E37" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="I37" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="M37" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="Q37" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="U37" s="0" t="n">
-        <v>35</v>
-      </c>
-      <c r="Y37" s="0" t="n">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="E38" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="I38" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="M38" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="Q38" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="U38" s="0" t="n">
-        <v>36</v>
-      </c>
-      <c r="Y38" s="0" t="n">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
-        <v>37</v>
-      </c>
-      <c r="E39" s="0" t="n">
-        <v>37</v>
-      </c>
-      <c r="I39" s="0" t="n">
-        <v>37</v>
-      </c>
-      <c r="M39" s="0" t="n">
-        <v>37</v>
-      </c>
-      <c r="Q39" s="0" t="n">
-        <v>37</v>
-      </c>
-      <c r="U39" s="0" t="n">
-        <v>37</v>
-      </c>
-      <c r="Y39" s="0" t="n">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="E40" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="I40" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="M40" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="Q40" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="U40" s="0" t="n">
-        <v>38</v>
-      </c>
-      <c r="Y40" s="0" t="n">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="E41" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="I41" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="M41" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="Q41" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="U41" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="Y41" s="0" t="n">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="E42" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="I42" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="M42" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="Q42" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="U42" s="0" t="n">
-        <v>40</v>
-      </c>
-      <c r="Y42" s="0" t="n">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="E43" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="I43" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="M43" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="Q43" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="U43" s="0" t="n">
-        <v>41</v>
-      </c>
-      <c r="Y43" s="0" t="n">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="E44" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="I44" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="M44" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="Q44" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="U44" s="0" t="n">
-        <v>42</v>
-      </c>
-      <c r="Y44" s="0" t="n">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="E45" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="I45" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="M45" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="Q45" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="U45" s="0" t="n">
-        <v>43</v>
-      </c>
-      <c r="Y45" s="0" t="n">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="E46" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="I46" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="M46" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="Q46" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="U46" s="0" t="n">
-        <v>44</v>
-      </c>
-      <c r="Y46" s="0" t="n">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="E47" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="I47" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="M47" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="Q47" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="U47" s="0" t="n">
-        <v>45</v>
-      </c>
-      <c r="Y47" s="0" t="n">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="E48" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="I48" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="M48" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="Q48" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="U48" s="0" t="n">
-        <v>46</v>
-      </c>
-      <c r="Y48" s="0" t="n">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="E49" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="I49" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="M49" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="Q49" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="U49" s="0" t="n">
-        <v>47</v>
-      </c>
-      <c r="Y49" s="0" t="n">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="E50" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="I50" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="M50" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="Q50" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="U50" s="0" t="n">
-        <v>48</v>
-      </c>
-      <c r="Y50" s="0" t="n">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="E51" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="I51" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="M51" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="Q51" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="U51" s="0" t="n">
-        <v>49</v>
-      </c>
-      <c r="Y51" s="0" t="n">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="E52" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="I52" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="M52" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="Q52" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="U52" s="0" t="n">
-        <v>50</v>
-      </c>
-      <c r="Y52" s="0" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
-        <v>51</v>
-      </c>
-      <c r="E53" s="0" t="n">
-        <v>51</v>
-      </c>
-      <c r="I53" s="0" t="n">
-        <v>51</v>
-      </c>
-      <c r="M53" s="0" t="n">
-        <v>51</v>
-      </c>
-      <c r="Q53" s="0" t="n">
-        <v>51</v>
-      </c>
-      <c r="U53" s="0" t="n">
-        <v>51</v>
-      </c>
-      <c r="Y53" s="0" t="n">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
-        <v>52</v>
-      </c>
-      <c r="E54" s="0" t="n">
-        <v>52</v>
-      </c>
-      <c r="I54" s="0" t="n">
-        <v>52</v>
-      </c>
-      <c r="M54" s="0" t="n">
-        <v>52</v>
-      </c>
-      <c r="Q54" s="0" t="n">
-        <v>52</v>
-      </c>
-      <c r="U54" s="0" t="n">
-        <v>52</v>
-      </c>
-      <c r="Y54" s="0" t="n">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="E55" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="I55" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="M55" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="Q55" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="U55" s="0" t="n">
-        <v>53</v>
-      </c>
-      <c r="Y55" s="0" t="n">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="n">
-        <v>54</v>
-      </c>
-      <c r="E56" s="0" t="n">
-        <v>54</v>
-      </c>
-      <c r="I56" s="0" t="n">
-        <v>54</v>
-      </c>
-      <c r="M56" s="0" t="n">
-        <v>54</v>
-      </c>
-      <c r="Q56" s="0" t="n">
-        <v>54</v>
-      </c>
-      <c r="U56" s="0" t="n">
-        <v>54</v>
-      </c>
-      <c r="Y56" s="0" t="n">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
-        <v>55</v>
-      </c>
-      <c r="E57" s="0" t="n">
-        <v>55</v>
-      </c>
-      <c r="I57" s="0" t="n">
-        <v>55</v>
-      </c>
-      <c r="M57" s="0" t="n">
-        <v>55</v>
-      </c>
-      <c r="Q57" s="0" t="n">
-        <v>55</v>
-      </c>
-      <c r="U57" s="0" t="n">
-        <v>55</v>
-      </c>
-      <c r="Y57" s="0" t="n">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="n">
-        <v>56</v>
-      </c>
-      <c r="E58" s="0" t="n">
-        <v>56</v>
-      </c>
-      <c r="I58" s="0" t="n">
-        <v>56</v>
-      </c>
-      <c r="M58" s="0" t="n">
-        <v>56</v>
-      </c>
-      <c r="Q58" s="0" t="n">
-        <v>56</v>
-      </c>
-      <c r="U58" s="0" t="n">
-        <v>56</v>
-      </c>
-      <c r="Y58" s="0" t="n">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
-        <v>57</v>
-      </c>
-      <c r="E59" s="0" t="n">
-        <v>57</v>
-      </c>
-      <c r="I59" s="0" t="n">
-        <v>57</v>
-      </c>
-      <c r="M59" s="0" t="n">
-        <v>57</v>
-      </c>
-      <c r="Q59" s="0" t="n">
-        <v>57</v>
-      </c>
-      <c r="U59" s="0" t="n">
-        <v>57</v>
-      </c>
-      <c r="Y59" s="0" t="n">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="n">
-        <v>58</v>
-      </c>
-      <c r="E60" s="0" t="n">
-        <v>58</v>
-      </c>
-      <c r="I60" s="0" t="n">
-        <v>58</v>
-      </c>
-      <c r="M60" s="0" t="n">
-        <v>58</v>
-      </c>
-      <c r="Q60" s="0" t="n">
-        <v>58</v>
-      </c>
-      <c r="U60" s="0" t="n">
-        <v>58</v>
-      </c>
-      <c r="Y60" s="0" t="n">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="E61" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="I61" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="M61" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="Q61" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="U61" s="0" t="n">
-        <v>59</v>
-      </c>
-      <c r="Y61" s="0" t="n">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="E62" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="I62" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="M62" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="Q62" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="U62" s="0" t="n">
-        <v>60</v>
-      </c>
-      <c r="Y62" s="0" t="n">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
-        <v>61</v>
-      </c>
-      <c r="E63" s="0" t="n">
-        <v>61</v>
-      </c>
-      <c r="I63" s="0" t="n">
-        <v>61</v>
-      </c>
-      <c r="M63" s="0" t="n">
-        <v>61</v>
-      </c>
-      <c r="Q63" s="0" t="n">
-        <v>61</v>
-      </c>
-      <c r="U63" s="0" t="n">
-        <v>61</v>
-      </c>
-      <c r="Y63" s="0" t="n">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
-        <v>62</v>
-      </c>
-      <c r="E64" s="0" t="n">
-        <v>62</v>
-      </c>
-      <c r="I64" s="0" t="n">
-        <v>62</v>
-      </c>
-      <c r="M64" s="0" t="n">
-        <v>62</v>
-      </c>
-      <c r="Q64" s="0" t="n">
-        <v>62</v>
-      </c>
-      <c r="U64" s="0" t="n">
-        <v>62</v>
-      </c>
-      <c r="Y64" s="0" t="n">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
-        <v>63</v>
-      </c>
-      <c r="E65" s="0" t="n">
-        <v>63</v>
-      </c>
-      <c r="I65" s="0" t="n">
-        <v>63</v>
-      </c>
-      <c r="M65" s="0" t="n">
-        <v>63</v>
-      </c>
-      <c r="Q65" s="0" t="n">
-        <v>63</v>
-      </c>
-      <c r="U65" s="0" t="n">
-        <v>63</v>
-      </c>
-      <c r="Y65" s="0" t="n">
-        <v>63</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -3572,1806 +2977,2065 @@
   </sheetPr>
   <dimension ref="A1:O212"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9:F12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="16.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="17.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="A1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="C1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="4" t="n">
         <v>14336</v>
       </c>
-      <c r="B2" s="0" t="str">
+      <c r="B2" s="4" t="str">
         <f aca="false">DEC2HEX(A2)</f>
         <v>3800</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
+      <c r="C2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="4" t="n">
         <v>14368</v>
       </c>
-      <c r="B3" s="0" t="str">
+      <c r="B3" s="4" t="str">
         <f aca="false">DEC2HEX(A3)</f>
         <v>3820</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="C3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="4" t="n">
         <v>14400</v>
       </c>
-      <c r="B4" s="0" t="str">
+      <c r="B4" s="4" t="str">
         <f aca="false">DEC2HEX(A4)</f>
         <v>3840</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
+      <c r="C4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="4" t="n">
         <v>14432</v>
       </c>
-      <c r="B5" s="0" t="str">
+      <c r="B5" s="4" t="str">
         <f aca="false">DEC2HEX(A5)</f>
         <v>3860</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="4" t="n">
         <v>14464</v>
       </c>
-      <c r="B6" s="0" t="str">
+      <c r="B6" s="4" t="str">
         <f aca="false">DEC2HEX(A6)</f>
         <v>3880</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="5"/>
+      <c r="C6" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+      <c r="A7" s="4" t="n">
         <v>14496</v>
       </c>
-      <c r="B7" s="0" t="str">
+      <c r="B7" s="4" t="str">
         <f aca="false">DEC2HEX(A7)</f>
         <v>38A0</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+      <c r="A8" s="4" t="n">
         <v>14528</v>
       </c>
-      <c r="B8" s="0" t="str">
+      <c r="B8" s="4" t="str">
         <f aca="false">DEC2HEX(A8)</f>
         <v>38C0</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="5"/>
-      <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="4" t="n">
         <v>14560</v>
       </c>
-      <c r="B9" s="0" t="str">
+      <c r="B9" s="4" t="str">
         <f aca="false">DEC2HEX(A9)</f>
         <v>38E0</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="5"/>
-      <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
+      <c r="A10" s="4" t="n">
         <v>14592</v>
       </c>
-      <c r="B10" s="0" t="str">
+      <c r="B10" s="4" t="str">
         <f aca="false">DEC2HEX(A10)</f>
         <v>3900</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="4" t="n">
         <v>14624</v>
       </c>
-      <c r="B11" s="0" t="str">
+      <c r="B11" s="4" t="str">
         <f aca="false">DEC2HEX(A11)</f>
         <v>3920</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
+      <c r="A12" s="4" t="n">
         <v>14656</v>
       </c>
-      <c r="B12" s="0" t="str">
+      <c r="B12" s="4" t="str">
         <f aca="false">DEC2HEX(A12)</f>
         <v>3940</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="5"/>
-      <c r="L12" s="5"/>
-      <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
+      <c r="A13" s="4" t="n">
         <v>14688</v>
       </c>
-      <c r="B13" s="0" t="str">
+      <c r="B13" s="4" t="str">
         <f aca="false">DEC2HEX(A13)</f>
         <v>3960</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="5"/>
-      <c r="L13" s="5"/>
-      <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="4" t="n">
         <v>14720</v>
       </c>
-      <c r="B14" s="0" t="str">
+      <c r="B14" s="4" t="str">
         <f aca="false">DEC2HEX(A14)</f>
         <v>3980</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
+      <c r="A15" s="4" t="n">
         <v>14752</v>
       </c>
-      <c r="B15" s="0" t="str">
+      <c r="B15" s="4" t="str">
         <f aca="false">DEC2HEX(A15)</f>
         <v>39A0</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="H15" s="4"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
+      <c r="A16" s="4" t="n">
         <v>14784</v>
       </c>
-      <c r="B16" s="0" t="str">
+      <c r="B16" s="4" t="str">
         <f aca="false">DEC2HEX(A16)</f>
         <v>39C0</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
-      <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
+      <c r="A17" s="4" t="n">
         <v>14816</v>
       </c>
-      <c r="B17" s="0" t="str">
+      <c r="B17" s="4" t="str">
         <f aca="false">DEC2HEX(A17)</f>
         <v>39E0</v>
       </c>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="3"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
+      <c r="A18" s="4" t="n">
         <v>14848</v>
       </c>
-      <c r="B18" s="0" t="str">
+      <c r="B18" s="4" t="str">
         <f aca="false">DEC2HEX(A18)</f>
         <v>3A00</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
+      <c r="A19" s="4" t="n">
         <v>14880</v>
       </c>
-      <c r="B19" s="0" t="str">
+      <c r="B19" s="4" t="str">
         <f aca="false">DEC2HEX(A19)</f>
         <v>3A20</v>
       </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
-      <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+      <c r="A20" s="4" t="n">
         <v>14912</v>
       </c>
-      <c r="B20" s="0" t="str">
+      <c r="B20" s="4" t="str">
         <f aca="false">DEC2HEX(A20)</f>
         <v>3A40</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
-      <c r="M20" s="5"/>
-      <c r="N20" s="5"/>
-      <c r="O20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="4" t="n">
         <v>14944</v>
       </c>
-      <c r="B21" s="0" t="str">
+      <c r="B21" s="4" t="str">
         <f aca="false">DEC2HEX(A21)</f>
         <v>3A60</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
-      <c r="N21" s="5"/>
-      <c r="O21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
+      <c r="A22" s="4" t="n">
         <v>14976</v>
       </c>
-      <c r="B22" s="0" t="str">
+      <c r="B22" s="4" t="str">
         <f aca="false">DEC2HEX(A22)</f>
         <v>3A80</v>
       </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
-      <c r="M22" s="5"/>
-      <c r="N22" s="5"/>
-      <c r="O22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
+      <c r="A23" s="4" t="n">
         <v>15008</v>
       </c>
-      <c r="B23" s="0" t="str">
+      <c r="B23" s="4" t="str">
         <f aca="false">DEC2HEX(A23)</f>
         <v>3AA0</v>
       </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
-      <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
-      <c r="O23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="n">
+      <c r="A24" s="4" t="n">
         <v>15040</v>
       </c>
-      <c r="B24" s="0" t="str">
+      <c r="B24" s="4" t="str">
         <f aca="false">DEC2HEX(A24)</f>
         <v>3AC0</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="5"/>
-      <c r="L24" s="5"/>
-      <c r="M24" s="5"/>
-      <c r="N24" s="5"/>
-      <c r="O24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
+      <c r="A25" s="4" t="n">
         <v>15072</v>
       </c>
-      <c r="B25" s="0" t="str">
+      <c r="B25" s="4" t="str">
         <f aca="false">DEC2HEX(A25)</f>
         <v>3AE0</v>
       </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="5"/>
-      <c r="L25" s="5"/>
-      <c r="M25" s="5"/>
-      <c r="N25" s="5"/>
-      <c r="O25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
+      <c r="A26" s="4" t="n">
         <v>15104</v>
       </c>
-      <c r="B26" s="0" t="str">
+      <c r="B26" s="4" t="str">
         <f aca="false">DEC2HEX(A26)</f>
         <v>3B00</v>
       </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="5"/>
-      <c r="L26" s="5"/>
-      <c r="M26" s="5"/>
-      <c r="N26" s="5"/>
-      <c r="O26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="J26" s="5"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+      <c r="A27" s="4" t="n">
         <v>15136</v>
       </c>
-      <c r="B27" s="0" t="str">
+      <c r="B27" s="4" t="str">
         <f aca="false">DEC2HEX(A27)</f>
         <v>3B20</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="5"/>
-      <c r="L27" s="5"/>
-      <c r="M27" s="5"/>
-      <c r="N27" s="5"/>
-      <c r="O27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="J27" s="5"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="n">
+      <c r="A28" s="4" t="n">
         <v>15168</v>
       </c>
-      <c r="B28" s="0" t="str">
+      <c r="B28" s="4" t="str">
         <f aca="false">DEC2HEX(A28)</f>
         <v>3B40</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="5"/>
-      <c r="L28" s="5"/>
-      <c r="M28" s="5"/>
-      <c r="N28" s="5"/>
-      <c r="O28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="J28" s="5"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="4" t="n">
         <v>15200</v>
       </c>
-      <c r="B29" s="0" t="str">
+      <c r="B29" s="4" t="str">
         <f aca="false">DEC2HEX(A29)</f>
         <v>3B60</v>
       </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="J29" s="5"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
+      <c r="A30" s="4" t="n">
         <v>15232</v>
       </c>
-      <c r="B30" s="0" t="str">
+      <c r="B30" s="4" t="str">
         <f aca="false">DEC2HEX(A30)</f>
         <v>3B80</v>
       </c>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3" t="s">
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="I30" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="5"/>
-      <c r="L30" s="5"/>
-      <c r="M30" s="5"/>
-      <c r="N30" s="5"/>
-      <c r="O30" s="5"/>
+      <c r="J30" s="5"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="4" t="n">
         <v>15264</v>
       </c>
-      <c r="B31" s="0" t="str">
+      <c r="B31" s="4" t="str">
         <f aca="false">DEC2HEX(A31)</f>
         <v>3BA0</v>
       </c>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="5"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="O31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="J31" s="5"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
+      <c r="A32" s="4" t="n">
         <v>15296</v>
       </c>
-      <c r="B32" s="0" t="str">
+      <c r="B32" s="4" t="str">
         <f aca="false">DEC2HEX(A32)</f>
         <v>3BC0</v>
       </c>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="5"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="O32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J32" s="5"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="4" t="n">
         <v>15328</v>
       </c>
-      <c r="B33" s="0" t="str">
+      <c r="B33" s="4" t="str">
         <f aca="false">DEC2HEX(A33)</f>
         <v>3BE0</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G33" s="3"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="O33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="J33" s="5"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="4" t="n">
         <v>15360</v>
       </c>
-      <c r="B34" s="0" t="str">
+      <c r="B34" s="4" t="str">
         <f aca="false">DEC2HEX(A34)</f>
         <v>3C00</v>
       </c>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="5"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="O34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="J34" s="5"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="4" t="n">
         <v>15392</v>
       </c>
-      <c r="B35" s="0" t="str">
+      <c r="B35" s="4" t="str">
         <f aca="false">DEC2HEX(A35)</f>
         <v>3C20</v>
       </c>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="O35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="J35" s="5"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="4" t="n">
         <v>15424</v>
       </c>
-      <c r="B36" s="0" t="str">
+      <c r="B36" s="4" t="str">
         <f aca="false">DEC2HEX(A36)</f>
         <v>3C40</v>
       </c>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="5"/>
-      <c r="N36" s="5"/>
-      <c r="O36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="J36" s="5"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="4" t="n">
         <v>15456</v>
       </c>
-      <c r="B37" s="0" t="str">
+      <c r="B37" s="4" t="str">
         <f aca="false">DEC2HEX(A37)</f>
         <v>3C60</v>
       </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
-      <c r="N37" s="5"/>
-      <c r="O37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="J37" s="5"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="7"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="7"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="n">
+      <c r="A38" s="4" t="n">
         <v>15488</v>
       </c>
-      <c r="B38" s="0" t="str">
+      <c r="B38" s="4" t="str">
         <f aca="false">DEC2HEX(A38)</f>
         <v>3C80</v>
       </c>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="5"/>
-      <c r="L38" s="5"/>
-      <c r="M38" s="5"/>
-      <c r="N38" s="5"/>
-      <c r="O38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="J38" s="5"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="4" t="n">
         <v>15520</v>
       </c>
-      <c r="B39" s="0" t="str">
+      <c r="B39" s="4" t="str">
         <f aca="false">DEC2HEX(A39)</f>
         <v>3CA0</v>
       </c>
-      <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="5"/>
-      <c r="L39" s="5"/>
-      <c r="M39" s="5"/>
-      <c r="N39" s="5"/>
-      <c r="O39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="J39" s="5"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="n">
+      <c r="A40" s="4" t="n">
         <v>15552</v>
       </c>
-      <c r="B40" s="0" t="str">
+      <c r="B40" s="4" t="str">
         <f aca="false">DEC2HEX(A40)</f>
         <v>3CC0</v>
       </c>
-      <c r="C40" s="3"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="5"/>
-      <c r="L40" s="5"/>
-      <c r="M40" s="5"/>
-      <c r="N40" s="5"/>
-      <c r="O40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J40" s="5"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
+      <c r="A41" s="4" t="n">
         <v>15584</v>
       </c>
-      <c r="B41" s="0" t="str">
+      <c r="B41" s="4" t="str">
         <f aca="false">DEC2HEX(A41)</f>
         <v>3CE0</v>
       </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="F41" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="5"/>
-      <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="J41" s="5"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="n">
+      <c r="A42" s="4" t="n">
         <v>15616</v>
       </c>
-      <c r="B42" s="0" t="str">
+      <c r="B42" s="4" t="str">
         <f aca="false">DEC2HEX(A42)</f>
         <v>3D00</v>
       </c>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="F42" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="5"/>
-      <c r="L42" s="5"/>
-      <c r="M42" s="5"/>
-      <c r="N42" s="5"/>
-      <c r="O42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
+      <c r="A43" s="4" t="n">
         <v>15648</v>
       </c>
-      <c r="B43" s="0" t="str">
+      <c r="B43" s="4" t="str">
         <f aca="false">DEC2HEX(A43)</f>
         <v>3D20</v>
       </c>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="F43" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="5"/>
-      <c r="L43" s="5"/>
-      <c r="M43" s="5"/>
-      <c r="N43" s="5"/>
-      <c r="O43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
+      <c r="A44" s="4" t="n">
         <v>15680</v>
       </c>
-      <c r="B44" s="0" t="str">
+      <c r="B44" s="4" t="str">
         <f aca="false">DEC2HEX(A44)</f>
         <v>3D40</v>
       </c>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="F44" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="5"/>
-      <c r="L44" s="5"/>
-      <c r="M44" s="5"/>
-      <c r="N44" s="5"/>
-      <c r="O44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="K44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
+      <c r="N44" s="7"/>
+      <c r="O44" s="7"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
+      <c r="A45" s="4" t="n">
         <v>15712</v>
       </c>
-      <c r="B45" s="0" t="str">
+      <c r="B45" s="4" t="str">
         <f aca="false">DEC2HEX(A45)</f>
         <v>3D60</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="5"/>
-      <c r="L45" s="5"/>
-      <c r="M45" s="5"/>
-      <c r="N45" s="5"/>
-      <c r="O45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="7"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
+      <c r="A46" s="4" t="n">
         <v>15744</v>
       </c>
-      <c r="B46" s="0" t="str">
+      <c r="B46" s="4" t="str">
         <f aca="false">DEC2HEX(A46)</f>
         <v>3D80</v>
       </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="5"/>
-      <c r="L46" s="5"/>
-      <c r="M46" s="5"/>
-      <c r="N46" s="5"/>
-      <c r="O46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="K46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
+      <c r="N46" s="7"/>
+      <c r="O46" s="7"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="n">
+      <c r="A47" s="4" t="n">
         <v>15776</v>
       </c>
-      <c r="B47" s="0" t="str">
+      <c r="B47" s="4" t="str">
         <f aca="false">DEC2HEX(A47)</f>
         <v>3DA0</v>
       </c>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="5"/>
-      <c r="M47" s="5"/>
-      <c r="N47" s="5"/>
-      <c r="O47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="7"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="7"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
+      <c r="A48" s="4" t="n">
         <v>15808</v>
       </c>
-      <c r="B48" s="0" t="str">
+      <c r="B48" s="4" t="str">
         <f aca="false">DEC2HEX(A48)</f>
         <v>3DC0</v>
       </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5"/>
-      <c r="M48" s="5"/>
-      <c r="N48" s="5"/>
-      <c r="O48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="K48" s="7"/>
+      <c r="L48" s="7"/>
+      <c r="M48" s="7"/>
+      <c r="N48" s="7"/>
+      <c r="O48" s="7"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
+      <c r="A49" s="4" t="n">
         <v>15840</v>
       </c>
-      <c r="B49" s="0" t="str">
+      <c r="B49" s="4" t="str">
         <f aca="false">DEC2HEX(A49)</f>
         <v>3DE0</v>
       </c>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="5"/>
-      <c r="L49" s="5"/>
-      <c r="M49" s="5"/>
-      <c r="N49" s="5"/>
-      <c r="O49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="7"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="7"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
+      <c r="A50" s="4" t="n">
         <v>15872</v>
       </c>
-      <c r="B50" s="0" t="str">
+      <c r="B50" s="4" t="str">
         <f aca="false">DEC2HEX(A50)</f>
         <v>3E00</v>
       </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="H50" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="5"/>
-      <c r="M50" s="5"/>
-      <c r="N50" s="5"/>
-      <c r="O50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+      <c r="K50" s="7"/>
+      <c r="L50" s="7"/>
+      <c r="M50" s="7"/>
+      <c r="N50" s="7"/>
+      <c r="O50" s="7"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+      <c r="A51" s="4" t="n">
         <v>15904</v>
       </c>
-      <c r="B51" s="0" t="str">
+      <c r="B51" s="4" t="str">
         <f aca="false">DEC2HEX(A51)</f>
         <v>3E20</v>
       </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="5"/>
-      <c r="L51" s="5"/>
-      <c r="M51" s="5"/>
-      <c r="N51" s="5"/>
-      <c r="O51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="7"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="7"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
+      <c r="A52" s="4" t="n">
         <v>15936</v>
       </c>
-      <c r="B52" s="0" t="str">
+      <c r="B52" s="4" t="str">
         <f aca="false">DEC2HEX(A52)</f>
         <v>3E40</v>
       </c>
-      <c r="C52" s="3"/>
-      <c r="D52" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H52" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="5"/>
-      <c r="L52" s="5"/>
-      <c r="M52" s="5"/>
-      <c r="N52" s="5"/>
-      <c r="O52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
+      <c r="G52" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H52" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+      <c r="K52" s="7"/>
+      <c r="L52" s="7"/>
+      <c r="M52" s="7"/>
+      <c r="N52" s="7"/>
+      <c r="O52" s="7"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
+      <c r="A53" s="4" t="n">
         <v>15968</v>
       </c>
-      <c r="B53" s="0" t="str">
+      <c r="B53" s="4" t="str">
         <f aca="false">DEC2HEX(A53)</f>
         <v>3E60</v>
       </c>
-      <c r="C53" s="3"/>
-      <c r="D53" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="H53" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="5"/>
-      <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
-      <c r="N53" s="5"/>
-      <c r="O53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="G53" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="7"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="7"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
+      <c r="A54" s="4" t="n">
         <v>16000</v>
       </c>
-      <c r="B54" s="0" t="str">
+      <c r="B54" s="4" t="str">
         <f aca="false">DEC2HEX(A54)</f>
         <v>3E80</v>
       </c>
-      <c r="C54" s="3"/>
-      <c r="D54" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="K54" s="5"/>
-      <c r="L54" s="5"/>
-      <c r="M54" s="5"/>
-      <c r="N54" s="5"/>
-      <c r="O54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="G54" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="H54" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="K54" s="7"/>
+      <c r="L54" s="7"/>
+      <c r="M54" s="7"/>
+      <c r="N54" s="7"/>
+      <c r="O54" s="7"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
+      <c r="A55" s="4" t="n">
         <v>16032</v>
       </c>
-      <c r="B55" s="0" t="str">
+      <c r="B55" s="4" t="str">
         <f aca="false">DEC2HEX(A55)</f>
         <v>3EA0</v>
       </c>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="H55" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="K55" s="5"/>
-      <c r="L55" s="5"/>
-      <c r="M55" s="5"/>
-      <c r="N55" s="5"/>
-      <c r="O55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E55" s="5"/>
+      <c r="F55" s="5"/>
+      <c r="G55" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H55" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="7"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="7"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="n">
+      <c r="A56" s="4" t="n">
         <v>16064</v>
       </c>
-      <c r="B56" s="0" t="str">
+      <c r="B56" s="4" t="str">
         <f aca="false">DEC2HEX(A56)</f>
         <v>3EC0</v>
       </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="K56" s="5"/>
-      <c r="L56" s="5"/>
-      <c r="M56" s="5"/>
-      <c r="N56" s="5"/>
-      <c r="O56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5"/>
+      <c r="G56" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I56" s="5"/>
+      <c r="J56" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="K56" s="7"/>
+      <c r="L56" s="7"/>
+      <c r="M56" s="7"/>
+      <c r="N56" s="7"/>
+      <c r="O56" s="7"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
+      <c r="A57" s="4" t="n">
         <v>16096</v>
       </c>
-      <c r="B57" s="0" t="str">
+      <c r="B57" s="4" t="str">
         <f aca="false">DEC2HEX(A57)</f>
         <v>3EE0</v>
       </c>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="H57" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="I57" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="J57" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="K57" s="5"/>
-      <c r="L57" s="5"/>
-      <c r="M57" s="5"/>
-      <c r="N57" s="5"/>
-      <c r="O57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E57" s="5"/>
+      <c r="F57" s="5"/>
+      <c r="G57" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="K57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="7"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="7"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="n">
+      <c r="A58" s="4" t="n">
         <v>16128</v>
       </c>
-      <c r="B58" s="0" t="str">
+      <c r="B58" s="4" t="str">
         <f aca="false">DEC2HEX(A58)</f>
         <v>3F00</v>
       </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F58" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G58" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H58" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="J58" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="K58" s="5"/>
-      <c r="L58" s="5"/>
-      <c r="M58" s="5"/>
-      <c r="N58" s="5"/>
-      <c r="O58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="J58" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="K58" s="7"/>
+      <c r="L58" s="7"/>
+      <c r="M58" s="7"/>
+      <c r="N58" s="7"/>
+      <c r="O58" s="7"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
+      <c r="A59" s="4" t="n">
         <v>16160</v>
       </c>
-      <c r="B59" s="0" t="str">
+      <c r="B59" s="4" t="str">
         <f aca="false">DEC2HEX(A59)</f>
         <v>3F20</v>
       </c>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F59" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="I59" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="J59" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="K59" s="5"/>
-      <c r="L59" s="5"/>
-      <c r="M59" s="5"/>
-      <c r="N59" s="5"/>
-      <c r="O59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="F59" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H59" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="I59" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="J59" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="7"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="7"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="n">
+      <c r="A60" s="4" t="n">
         <v>16192</v>
       </c>
-      <c r="B60" s="0" t="str">
+      <c r="B60" s="4" t="str">
         <f aca="false">DEC2HEX(A60)</f>
         <v>3F40</v>
       </c>
-      <c r="C60" s="3"/>
-      <c r="D60" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="F60" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="H60" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="I60" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="J60" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="K60" s="5"/>
-      <c r="L60" s="5"/>
-      <c r="M60" s="5"/>
-      <c r="N60" s="5"/>
-      <c r="O60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F60" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="K60" s="7"/>
+      <c r="L60" s="7"/>
+      <c r="M60" s="7"/>
+      <c r="N60" s="7"/>
+      <c r="O60" s="7"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
+      <c r="A61" s="4" t="n">
         <v>16224</v>
       </c>
-      <c r="B61" s="0" t="str">
+      <c r="B61" s="4" t="str">
         <f aca="false">DEC2HEX(A61)</f>
         <v>3F60</v>
       </c>
-      <c r="C61" s="3"/>
-      <c r="D61" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="F61" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="G61" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H61" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="I61" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="J61" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="K61" s="5"/>
-      <c r="L61" s="5"/>
-      <c r="M61" s="5"/>
-      <c r="N61" s="5"/>
-      <c r="O61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E61" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F61" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="7"/>
+      <c r="N61" s="7"/>
+      <c r="O61" s="7"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
+      <c r="A62" s="4" t="n">
         <v>16256</v>
       </c>
-      <c r="B62" s="0" t="str">
+      <c r="B62" s="4" t="str">
         <f aca="false">DEC2HEX(A62)</f>
         <v>3F80</v>
       </c>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="E62" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="F62" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G62" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="H62" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="I62" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="J62" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="K62" s="5"/>
-      <c r="L62" s="5"/>
-      <c r="M62" s="5"/>
-      <c r="N62" s="5"/>
-      <c r="O62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="K62" s="7"/>
+      <c r="L62" s="7"/>
+      <c r="M62" s="7"/>
+      <c r="N62" s="7"/>
+      <c r="O62" s="7"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
+      <c r="A63" s="4" t="n">
         <v>16288</v>
       </c>
-      <c r="B63" s="0" t="str">
+      <c r="B63" s="4" t="str">
         <f aca="false">DEC2HEX(A63)</f>
         <v>3FA0</v>
       </c>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="G63" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="H63" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="J63" s="3" t="s">
-        <v>170</v>
-      </c>
-      <c r="K63" s="5"/>
-      <c r="L63" s="5"/>
-      <c r="M63" s="5"/>
-      <c r="N63" s="5"/>
-      <c r="O63" s="5"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="7"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="7"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
+      <c r="A64" s="4" t="n">
         <v>16320</v>
       </c>
-      <c r="B64" s="0" t="str">
+      <c r="B64" s="4" t="str">
         <f aca="false">DEC2HEX(A64)</f>
         <v>3FC0</v>
       </c>
-      <c r="C64" s="3"/>
-      <c r="D64" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="F64" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="G64" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="H64" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="I64" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="J64" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="K64" s="5"/>
-      <c r="L64" s="5"/>
-      <c r="M64" s="5"/>
-      <c r="N64" s="5"/>
-      <c r="O64" s="5"/>
+      <c r="C64" s="5"/>
+      <c r="D64" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="K64" s="7"/>
+      <c r="L64" s="7"/>
+      <c r="M64" s="7"/>
+      <c r="N64" s="7"/>
+      <c r="O64" s="7"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="n">
+      <c r="A65" s="4" t="n">
         <v>16352</v>
       </c>
-      <c r="B65" s="0" t="str">
+      <c r="B65" s="4" t="str">
         <f aca="false">DEC2HEX(A65)</f>
         <v>3FE0</v>
       </c>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="H65" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="I65" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="J65" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="K65" s="5"/>
-      <c r="L65" s="5"/>
-      <c r="M65" s="5"/>
-      <c r="N65" s="5"/>
-      <c r="O65" s="5"/>
+      <c r="C65" s="5"/>
+      <c r="D65" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="7"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="7"/>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B212" s="6"/>
+      <c r="B212" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Creadas funciones carga patrones
No estaban... 
Se continua con el proyecto
</commit_message>
<xml_diff>
--- a/doc/análisis posición en memoria sprites enemigos.xlsx
+++ b/doc/análisis posición en memoria sprites enemigos.xlsx
@@ -1230,10 +1230,10 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="1" sqref="F9:F65 L9"/>
+      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.07"/>
@@ -1926,10 +1926,10 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="1" sqref="F9:F65 B13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2093,10 +2093,10 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="1" sqref="F9:F65 B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.65"/>
   </cols>
@@ -2296,10 +2296,10 @@
   <dimension ref="A1:AA33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="F9:F65 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.92"/>
@@ -3350,10 +3350,10 @@
   <dimension ref="A1:AJ212"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F9" activeCellId="0" sqref="F9:F65"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.16"/>
@@ -8833,10 +8833,10 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="1" sqref="F9:F65 E9"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="5.32"/>

</xml_diff>

<commit_message>
Inicio eneigo jefe beholder y más
Inicio eneigo jefe beholder
Modificación funciones esqueleto (se elimina la Función actualiza valores para inicializar)
Se terminan los enemigos de los niveles del nivel 5
</commit_message>
<xml_diff>
--- a/doc/análisis posición en memoria sprites enemigos.xlsx
+++ b/doc/análisis posición en memoria sprites enemigos.xlsx
@@ -1350,10 +1350,10 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+      <selection pane="topLeft" activeCell="L9" activeCellId="1" sqref="Y26:Y33 L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.07"/>
@@ -2046,10 +2046,10 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B13" activeCellId="1" sqref="Y26:Y33 B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -2213,10 +2213,10 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+      <selection pane="topLeft" activeCell="B22" activeCellId="1" sqref="Y26:Y33 B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.65"/>
   </cols>
@@ -2416,10 +2416,10 @@
   <dimension ref="A1:AA33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="Y26:Y33 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="2.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="10.92"/>
@@ -3469,11 +3469,11 @@
   </sheetPr>
   <dimension ref="A1:AJ212"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F58" activeCellId="0" sqref="F58"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y26" activeCellId="0" sqref="Y26:Y33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="13.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.16"/>
@@ -5725,8 +5725,8 @@
         <v>82</v>
       </c>
       <c r="X26" s="10"/>
-      <c r="Y26" s="12" t="s">
-        <v>114</v>
+      <c r="Y26" s="5" t="s">
+        <v>145</v>
       </c>
       <c r="Z26" s="10" t="s">
         <v>143</v>
@@ -5810,8 +5810,8 @@
         <v>89</v>
       </c>
       <c r="X27" s="10"/>
-      <c r="Y27" s="12" t="s">
-        <v>118</v>
+      <c r="Y27" s="5" t="s">
+        <v>148</v>
       </c>
       <c r="Z27" s="10" t="s">
         <v>146</v>
@@ -5891,8 +5891,8 @@
       </c>
       <c r="W28" s="10"/>
       <c r="X28" s="10"/>
-      <c r="Y28" s="12" t="s">
-        <v>121</v>
+      <c r="Y28" s="5" t="s">
+        <v>151</v>
       </c>
       <c r="Z28" s="10" t="s">
         <v>149</v>
@@ -5972,8 +5972,8 @@
       </c>
       <c r="W29" s="10"/>
       <c r="X29" s="10"/>
-      <c r="Y29" s="12" t="s">
-        <v>125</v>
+      <c r="Y29" s="5" t="s">
+        <v>153</v>
       </c>
       <c r="Z29" s="10" t="s">
         <v>80</v>
@@ -6053,8 +6053,8 @@
       </c>
       <c r="W30" s="10"/>
       <c r="X30" s="10"/>
-      <c r="Y30" s="12" t="s">
-        <v>128</v>
+      <c r="Y30" s="5" t="s">
+        <v>156</v>
       </c>
       <c r="Z30" s="10" t="s">
         <v>154</v>
@@ -6134,8 +6134,8 @@
       </c>
       <c r="W31" s="10"/>
       <c r="X31" s="10"/>
-      <c r="Y31" s="12" t="s">
-        <v>132</v>
+      <c r="Y31" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="Z31" s="10" t="s">
         <v>157</v>
@@ -6215,8 +6215,8 @@
       </c>
       <c r="W32" s="10"/>
       <c r="X32" s="10"/>
-      <c r="Y32" s="12" t="s">
-        <v>136</v>
+      <c r="Y32" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="Z32" s="10" t="s">
         <v>160</v>
@@ -6296,8 +6296,8 @@
       </c>
       <c r="W33" s="10"/>
       <c r="X33" s="10"/>
-      <c r="Y33" s="12" t="s">
-        <v>140</v>
+      <c r="Y33" s="5" t="s">
+        <v>164</v>
       </c>
       <c r="Z33" s="10" t="s">
         <v>83</v>
@@ -8953,10 +8953,10 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="1" sqref="Y26:Y33 E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="5.32"/>
@@ -9184,10 +9184,10 @@
   <dimension ref="A1:AM25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AM4" activeCellId="0" sqref="AM4"/>
+      <selection pane="topLeft" activeCell="AM4" activeCellId="1" sqref="Y26:Y33 AM4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="0" width="2.54"/>
@@ -10343,10 +10343,10 @@
   <dimension ref="A1:AG25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AI7" activeCellId="0" sqref="AI7"/>
+      <selection pane="topLeft" activeCell="AI7" activeCellId="1" sqref="Y26:Y33 AI7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="2" style="0" width="2.54"/>

</xml_diff>